<commit_message>
Page Object Model 2025
</commit_message>
<xml_diff>
--- a/src/test/resources/com/pom/excel/testdata.xlsx
+++ b/src/test/resources/com/pom/excel/testdata.xlsx
@@ -1,42 +1,50 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspaces\BatchSeleniumSep2021\DataDrivenFramework\src\test\resources\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\seleniumworkspaces\LiveProjects\PageObjectModelBasics\src\test\resources\com\w2a\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9508F08B-CFB1-4675-A167-9B61E63C54B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="4215" windowWidth="21600" windowHeight="11385" activeTab="4" xr2:uid="{D68EBB81-B61C-4DDA-9343-37D6858EAB7B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17205" windowHeight="5370" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="LoginTest" sheetId="1" r:id="rId1"/>
-    <sheet name="doLogin" sheetId="2" r:id="rId2"/>
-    <sheet name="registerUser" sheetId="3" r:id="rId3"/>
-    <sheet name="addCustomer" sheetId="4" r:id="rId4"/>
-    <sheet name="openAccount" sheetId="5" r:id="rId5"/>
+    <sheet name="test_suite" sheetId="3" r:id="rId1"/>
+    <sheet name="LoginTest" sheetId="1" r:id="rId2"/>
+    <sheet name="CreateAccountTest" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+  <si>
+    <t>Raman</t>
+  </si>
+  <si>
+    <t>TCID</t>
+  </si>
+  <si>
+    <t>Runmode</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>runmode</t>
+  </si>
+  <si>
+    <t>LoginTest</t>
+  </si>
   <si>
     <t>username</t>
   </si>
@@ -47,82 +55,19 @@
     <t>trainer@way2automation.com</t>
   </si>
   <si>
-    <t>java@way2automation.com</t>
-  </si>
-  <si>
-    <t>dfsfds</t>
-  </si>
-  <si>
-    <t>jhgjhj</t>
-  </si>
-  <si>
-    <t>corporate@way2automation.com</t>
-  </si>
-  <si>
-    <t>sdfsdf</t>
-  </si>
-  <si>
-    <t>info@way2automation.com</t>
-  </si>
-  <si>
-    <t>sdfd</t>
-  </si>
-  <si>
-    <t>sdfsf</t>
-  </si>
-  <si>
-    <t>firstname</t>
-  </si>
-  <si>
-    <t>lastname</t>
-  </si>
-  <si>
-    <t>Rahul</t>
-  </si>
-  <si>
-    <t>Arora</t>
-  </si>
-  <si>
-    <t>postcode</t>
-  </si>
-  <si>
-    <t>A34234</t>
-  </si>
-  <si>
-    <t>Cory</t>
-  </si>
-  <si>
-    <t>Paul</t>
-  </si>
-  <si>
-    <t>S3434</t>
-  </si>
-  <si>
-    <t>Aryan</t>
-  </si>
-  <si>
-    <t>Khan</t>
-  </si>
-  <si>
-    <t>S23434</t>
-  </si>
-  <si>
-    <t>customer</t>
-  </si>
-  <si>
-    <t>currency</t>
-  </si>
-  <si>
-    <t>Rahul Arora</t>
-  </si>
-  <si>
-    <t>Rupee</t>
+    <t>Selenium@123</t>
+  </si>
+  <si>
+    <t>CreateAccountTest</t>
+  </si>
+  <si>
+    <t>accountname</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -199,7 +144,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -211,7 +156,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -228,9 +173,9 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -258,31 +203,14 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -310,23 +238,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -478,124 +389,37 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7A48967-B7F5-48DE-8B0F-B094AB22FF90}">
-  <dimension ref="A1:B5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{346F301B-B3E3-4DA8-9F6B-332A9B2B03EA}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{668160D6-385E-451C-A99B-60149CF4F6D9}"/>
-    <hyperlink ref="A4" r:id="rId3" xr:uid="{171009F4-6D14-4BEB-9BA1-5EE58148AA23}"/>
-    <hyperlink ref="A5" r:id="rId4" xr:uid="{D1861D8F-D479-43AA-88FA-9B75E0BE039C}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01898195-8D9B-493F-8670-3BD1CED4B146}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{A38B800B-F0E5-4D03-8466-403E031B8F3D}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DFF9B5F-70C0-44C9-8CDB-4F60CB1CC394}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -603,89 +427,65 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84E4CF94-55AD-4525-9EA3-ED9CD93EE9E1}">
-  <dimension ref="A1:C4"/>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" t="s">
-        <v>14</v>
+      <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" t="s">
-        <v>22</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7738BEC3-AA34-4F1A-A42F-F58C443139B5}">
-  <dimension ref="A1:B2"/>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" t="s">
-        <v>26</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>